<commit_message>
add study6~7 for simple glm and RF without text bag
</commit_message>
<xml_diff>
--- a/kaggleCompetition/指标.xlsx
+++ b/kaggleCompetition/指标.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>simple tree</t>
   </si>
@@ -45,6 +45,57 @@
   </si>
   <si>
     <t>valid accurracy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionCARTBag</t>
+  </si>
+  <si>
+    <t>SubmissionCARTSimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionLogBag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionLogSimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionRFBag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionRFSimple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionSimplestLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glm:WordCount+Weekday+Hour</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glm:WordCount+Weekday+Hour+NewsDesk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>glm:WordCount+Weekday+Hour+NewsDesk+SectionName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionSimplestRF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF: WordCount+NewsDesk+Hour+Weekday+SectionName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF: WordCount+NewsDesk+Hour+Weekday</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -53,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="0.00000_ "/>
+    <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -115,7 +166,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -128,10 +179,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -428,21 +482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>6</v>
@@ -454,7 +509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -467,8 +522,11 @@
       <c r="D2" s="4">
         <v>0.94373130000000005</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -481,8 +539,11 @@
       <c r="D3" s="4">
         <v>0.93567529999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -495,8 +556,11 @@
       <c r="D4" s="5">
         <v>0.933361</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -509,20 +573,28 @@
       <c r="D5" s="5">
         <v>0.92900000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>0.61426000000000003</v>
+      </c>
       <c r="C6" s="2">
         <v>0.90765309999999999</v>
       </c>
       <c r="D6" s="4">
         <v>0.90374860000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -534,6 +606,91 @@
       </c>
       <c r="D7" s="4">
         <v>0.89534389999999997</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>0.70491999999999999</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.83265310000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.73701320000000003</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>0.88571</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.87704079999999995</v>
+      </c>
+      <c r="D10">
+        <v>0.89479390000000003</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0.89671000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.89744900000000005</v>
+      </c>
+      <c r="D11">
+        <v>0.91554760000000002</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>0.91107000000000005</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.89795919999999996</v>
+      </c>
+      <c r="D12">
+        <v>0.91921189999999997</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.91326529999999995</v>
+      </c>
+      <c r="D13">
+        <v>0.93647460000000005</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update compitition with gbm
</commit_message>
<xml_diff>
--- a/kaggleCompetition/指标.xlsx
+++ b/kaggleCompetition/指标.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
   <si>
     <t>simple tree</t>
   </si>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
@@ -441,7 +441,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -460,9 +460,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -478,10 +475,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -499,7 +496,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -573,7 +570,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -608,7 +604,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -784,12 +779,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -847,37 +842,37 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="7" customFormat="1">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:6" s="6" customFormat="1">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>0.62870000000000004</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>0.90969390000000006</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>0.933361</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="7" customFormat="1">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:6" s="6" customFormat="1">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>0.62412999999999996</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>0.91377549999999996</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>0.92900000000000005</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -931,7 +926,7 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -951,7 +946,7 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
@@ -969,7 +964,7 @@
       <c r="E11" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -987,7 +982,7 @@
       <c r="E12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -1005,7 +1000,7 @@
       <c r="E13" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
@@ -1015,50 +1010,58 @@
         <v>0.92652999999999996</v>
       </c>
       <c r="C14" s="1">
-        <v>0.91275510000000004</v>
+        <v>0.91377549999999996</v>
       </c>
       <c r="D14" s="1">
-        <v>0.93629879999999999</v>
+        <v>0.93660869999999996</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" s="7" customFormat="1">
-      <c r="A15" s="7" t="s">
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1">
+      <c r="A15" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>0.92410000000000003</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.91581630000000003</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>0.93785719999999995</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" s="7" customFormat="1">
-      <c r="A16" s="7" t="s">
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1">
+      <c r="A16" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="7">
+      <c r="B16">
+        <v>0.92637000000000003</v>
+      </c>
+      <c r="C16" s="6">
         <v>0.91377549999999996</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>0.93753889999999995</v>
       </c>
-      <c r="F16" s="13"/>
+      <c r="E16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>103</v>
+      </c>
+      <c r="B17">
+        <v>0.92430000000000001</v>
       </c>
       <c r="C17">
         <v>0.91530610000000001</v>
@@ -1066,9 +1069,12 @@
       <c r="D17">
         <v>0.93518920000000005</v>
       </c>
+      <c r="E17" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
@@ -1091,7 +1097,7 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="7">
         <v>0.91571999999999998</v>
       </c>
       <c r="C20">
@@ -1126,7 +1132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -1136,17 +1142,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="77.125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="77.125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1156,12 +1162,12 @@
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1171,72 +1177,72 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:1" s="9" customFormat="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:1" s="8" customFormat="1">
+      <c r="A8" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1248,7 +1254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A53"/>
   <sheetViews>
@@ -1258,86 +1264,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="78.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.25" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="7" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" s="6" customFormat="1">
+      <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1347,182 +1353,182 @@
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="6" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="6" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="6" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="6" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="6" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="6" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="6" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="6" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="6" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="6" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update competition: combine 2 model
</commit_message>
<xml_diff>
--- a/kaggleCompetition/指标.xlsx
+++ b/kaggleCompetition/指标.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>simple tree</t>
   </si>
@@ -103,260 +103,271 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionBagAbstractRF.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract), ntree = 800, nodesize=7</t>
+  </si>
+  <si>
+    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract), ntree = 800, nodesize=11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[1] "ntree =  100 : acc= 0.913265306122449 , auc= 0.928979480511717"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  200 : acc= 0.913265306122449 , auc= 0.932023590686274"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  300 : acc= 0.914285714285714 , auc= 0.931348263390722"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  400 : acc= 0.913775510204082 , auc= 0.931938590985175"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  500 : acc= 0.913775510204082 , auc= 0.932118865076518"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  600 : acc= 0.913775510204082 , auc= 0.93357693687231"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  700 : acc= 0.912755102040816 , auc= 0.933264959947393"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  800 : acc= 0.912244897959184 , auc= 0.933191168998087"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  900 : acc= 0.913265306122449 , auc= 0.933105235234338"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1000 : acc= 0.913775510204082 , auc= 0.932873587697274"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1100 : acc= 0.914285714285714 , auc= 0.932885730511717"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1200 : acc= 0.914285714285714 , auc= 0.932736280487805"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1300 : acc= 0.913265306122449 , auc= 0.932592434839789"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1400 : acc= 0.913775510204082 , auc= 0.932363589490674"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1500 : acc= 0.913775510204082 , auc= 0.932357985114777"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1600 : acc= 0.913265306122449 , auc= 0.932216007592061"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1700 : acc= 0.913265306122449 , auc= 0.932100183823529"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1800 : acc= 0.913265306122449 , auc= 0.932049744440459"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  1900 : acc= 0.913265306122449 , auc= 0.931921777857485"</t>
+  </si>
+  <si>
+    <t>[1] "ntree =  2000 : acc= 0.913775510204082 , auc= 0.931796613462458"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  48 : acc= 0.911734693877551 , auc= 0.923490928383549"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  49 : acc= 0.910204081632653 , auc= 0.924025212219034"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  50 : acc= 0.910714285714286 , auc= 0.924234442252511"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  1 : acc= 0.913775510204082 , auc= 0.93357693687231"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  2 : acc= 0.915816326530612 , auc= 0.933394794655667"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  3 : acc= 0.913265306122449 , auc= 0.92854887763032"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  4 : acc= 0.914795918367347 , auc= 0.931837712219034"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  5 : acc= 0.913265306122449 , auc= 0.93269424766858"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  6 : acc= 0.914795918367347 , auc= 0.932261776661884"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  7 : acc= 0.913265306122449 , auc= 0.932635401721664"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  8 : acc= 0.912755102040816 , auc= 0.931936722859876"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  9 : acc= 0.91530612244898 , auc= 0.932042271939264"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  10 : acc= 0.913775510204082 , auc= 0.932061887254902"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  11 : acc= 0.914285714285714 , auc= 0.931863865973218"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  12 : acc= 0.91530612244898 , auc= 0.932126337577714"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  13 : acc= 0.913265306122449 , auc= 0.932655951099952"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  14 : acc= 0.914285714285714 , auc= 0.929113985533238"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  15 : acc= 0.914285714285714 , auc= 0.932952983022477"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  16 : acc= 0.912755102040816 , auc= 0.931636888749402"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  17 : acc= 0.91530612244898 , auc= 0.934440010760402"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  18 : acc= 0.913775510204082 , auc= 0.930575793579627"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  19 : acc= 0.914285714285714 , auc= 0.930182553204209"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  20 : acc= 0.914285714285714 , auc= 0.930082608500717"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  21 : acc= 0.914285714285714 , auc= 0.931254857125777"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  22 : acc= 0.913265306122449 , auc= 0.931003594273075"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  23 : acc= 0.913775510204082 , auc= 0.930686947034912"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  24 : acc= 0.913775510204082 , auc= 0.92956887404352"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  25 : acc= 0.913775510204082 , auc= 0.930115300693448"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  26 : acc= 0.913775510204082 , auc= 0.930014421927308"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  27 : acc= 0.914285714285714 , auc= 0.930130245695839"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  28 : acc= 0.91530612244898 , auc= 0.929762225011956"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  29 : acc= 0.913775510204082 , auc= 0.929395138390722"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  30 : acc= 0.914285714285714 , auc= 0.92686849892396"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  31 : acc= 0.914285714285714 , auc= 0.928146296628408"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  32 : acc= 0.91530612244898 , auc= 0.928377010102822"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  33 : acc= 0.914285714285714 , auc= 0.926418280726925"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  34 : acc= 0.914795918367347 , auc= 0.925869051889048"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  35 : acc= 0.913775510204082 , auc= 0.928292944464371"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  36 : acc= 0.914285714285714 , auc= 0.927895967838355"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  37 : acc= 0.913775510204082 , auc= 0.926252951637972"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  38 : acc= 0.914795918367347 , auc= 0.924058838474414"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  39 : acc= 0.911734693877551 , auc= 0.925008780188905"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  40 : acc= 0.914285714285714 , auc= 0.924769660150646"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  41 : acc= 0.913775510204082 , auc= 0.926591082317073"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  42 : acc= 0.914285714285714 , auc= 0.922609173242468"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  43 : acc= 0.912755102040816 , auc= 0.923584334648493"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  44 : acc= 0.913775510204082 , auc= 0.925588833094213"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  45 : acc= 0.913775510204082 , auc= 0.926791905786705"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  46 : acc= 0.911224489795918 , auc= 0.923856146879483"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  47 : acc= 0.910714285714286 , auc= 0.927172069285031"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  48 : acc= 0.910714285714286 , auc= 0.924432463534194"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  49 : acc= 0.911224489795918 , auc= 0.920603740734098"</t>
+  </si>
+  <si>
+    <t>[1] "nodesize =  50 : acc= 0.908673469387755 , auc= 0.925616854973697"</t>
+  </si>
+  <si>
+    <t>RF: WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName, ntree = 800, nodesize=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF: log(WordCount+1)+NewsDesk+Hour+Weekday+SectionName+SubsectionName, ntree = 600, nodesize=17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RF: log(WordCount+1)+NewsDesk+Hour+Weekday+SectionName+SubsectionName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SubmissionLogRF.csv</t>
+  </si>
+  <si>
+    <t>study9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>RF: WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SubmissionBagAbstractRF.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract), ntree = 800, nodesize=7</t>
-  </si>
-  <si>
-    <t>RF:WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName+bag(Abstract), ntree = 800, nodesize=11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[1] "ntree =  100 : acc= 0.913265306122449 , auc= 0.928979480511717"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  200 : acc= 0.913265306122449 , auc= 0.932023590686274"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  300 : acc= 0.914285714285714 , auc= 0.931348263390722"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  400 : acc= 0.913775510204082 , auc= 0.931938590985175"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  500 : acc= 0.913775510204082 , auc= 0.932118865076518"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  600 : acc= 0.913775510204082 , auc= 0.93357693687231"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  700 : acc= 0.912755102040816 , auc= 0.933264959947393"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  800 : acc= 0.912244897959184 , auc= 0.933191168998087"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  900 : acc= 0.913265306122449 , auc= 0.933105235234338"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1000 : acc= 0.913775510204082 , auc= 0.932873587697274"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1100 : acc= 0.914285714285714 , auc= 0.932885730511717"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1200 : acc= 0.914285714285714 , auc= 0.932736280487805"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1300 : acc= 0.913265306122449 , auc= 0.932592434839789"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1400 : acc= 0.913775510204082 , auc= 0.932363589490674"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1500 : acc= 0.913775510204082 , auc= 0.932357985114777"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1600 : acc= 0.913265306122449 , auc= 0.932216007592061"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1700 : acc= 0.913265306122449 , auc= 0.932100183823529"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1800 : acc= 0.913265306122449 , auc= 0.932049744440459"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  1900 : acc= 0.913265306122449 , auc= 0.931921777857485"</t>
-  </si>
-  <si>
-    <t>[1] "ntree =  2000 : acc= 0.913775510204082 , auc= 0.931796613462458"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  48 : acc= 0.911734693877551 , auc= 0.923490928383549"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  49 : acc= 0.910204081632653 , auc= 0.924025212219034"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  50 : acc= 0.910714285714286 , auc= 0.924234442252511"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  1 : acc= 0.913775510204082 , auc= 0.93357693687231"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  2 : acc= 0.915816326530612 , auc= 0.933394794655667"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  3 : acc= 0.913265306122449 , auc= 0.92854887763032"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  4 : acc= 0.914795918367347 , auc= 0.931837712219034"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  5 : acc= 0.913265306122449 , auc= 0.93269424766858"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  6 : acc= 0.914795918367347 , auc= 0.932261776661884"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  7 : acc= 0.913265306122449 , auc= 0.932635401721664"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  8 : acc= 0.912755102040816 , auc= 0.931936722859876"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  9 : acc= 0.91530612244898 , auc= 0.932042271939264"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  10 : acc= 0.913775510204082 , auc= 0.932061887254902"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  11 : acc= 0.914285714285714 , auc= 0.931863865973218"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  12 : acc= 0.91530612244898 , auc= 0.932126337577714"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  13 : acc= 0.913265306122449 , auc= 0.932655951099952"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  14 : acc= 0.914285714285714 , auc= 0.929113985533238"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  15 : acc= 0.914285714285714 , auc= 0.932952983022477"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  16 : acc= 0.912755102040816 , auc= 0.931636888749402"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  17 : acc= 0.91530612244898 , auc= 0.934440010760402"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  18 : acc= 0.913775510204082 , auc= 0.930575793579627"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  19 : acc= 0.914285714285714 , auc= 0.930182553204209"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  20 : acc= 0.914285714285714 , auc= 0.930082608500717"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  21 : acc= 0.914285714285714 , auc= 0.931254857125777"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  22 : acc= 0.913265306122449 , auc= 0.931003594273075"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  23 : acc= 0.913775510204082 , auc= 0.930686947034912"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  24 : acc= 0.913775510204082 , auc= 0.92956887404352"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  25 : acc= 0.913775510204082 , auc= 0.930115300693448"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  26 : acc= 0.913775510204082 , auc= 0.930014421927308"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  27 : acc= 0.914285714285714 , auc= 0.930130245695839"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  28 : acc= 0.91530612244898 , auc= 0.929762225011956"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  29 : acc= 0.913775510204082 , auc= 0.929395138390722"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  30 : acc= 0.914285714285714 , auc= 0.92686849892396"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  31 : acc= 0.914285714285714 , auc= 0.928146296628408"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  32 : acc= 0.91530612244898 , auc= 0.928377010102822"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  33 : acc= 0.914285714285714 , auc= 0.926418280726925"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  34 : acc= 0.914795918367347 , auc= 0.925869051889048"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  35 : acc= 0.913775510204082 , auc= 0.928292944464371"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  36 : acc= 0.914285714285714 , auc= 0.927895967838355"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  37 : acc= 0.913775510204082 , auc= 0.926252951637972"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  38 : acc= 0.914795918367347 , auc= 0.924058838474414"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  39 : acc= 0.911734693877551 , auc= 0.925008780188905"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  40 : acc= 0.914285714285714 , auc= 0.924769660150646"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  41 : acc= 0.913775510204082 , auc= 0.926591082317073"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  42 : acc= 0.914285714285714 , auc= 0.922609173242468"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  43 : acc= 0.912755102040816 , auc= 0.923584334648493"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  44 : acc= 0.913775510204082 , auc= 0.925588833094213"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  45 : acc= 0.913775510204082 , auc= 0.926791905786705"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  46 : acc= 0.911224489795918 , auc= 0.923856146879483"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  47 : acc= 0.910714285714286 , auc= 0.927172069285031"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  48 : acc= 0.910714285714286 , auc= 0.924432463534194"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  49 : acc= 0.911224489795918 , auc= 0.920603740734098"</t>
-  </si>
-  <si>
-    <t>[1] "nodesize =  50 : acc= 0.908673469387755 , auc= 0.925616854973697"</t>
-  </si>
-  <si>
-    <t>RF: log(WordCount+1)+NewsDesk+Hour+Weekday+SectionName+SubsectionName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RF: WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName, ntree = 800, nodesize=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RF: log(WordCount+1)+NewsDesk+Hour+Weekday+SectionName+SubsectionName, ntree = 600, nodesize=17</t>
+    <t>(glm+RF)/2:  WordCount+NewsDesk+Hour+Weekday+SectionName+SubsectionName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
@@ -496,7 +507,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -570,6 +581,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -604,6 +616,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -779,12 +792,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1004,7 +1017,7 @@
     </row>
     <row r="14" spans="1:6" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="B14" s="1">
         <v>0.92652999999999996</v>
@@ -1022,7 +1035,7 @@
     </row>
     <row r="15" spans="1:6" s="6" customFormat="1">
       <c r="A15" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15">
         <v>0.92410000000000003</v>
@@ -1040,7 +1053,7 @@
     </row>
     <row r="16" spans="1:6" s="6" customFormat="1">
       <c r="A16" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B16">
         <v>0.92637000000000003</v>
@@ -1056,9 +1069,9 @@
       </c>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17">
         <v>0.92430000000000001</v>
@@ -1073,12 +1086,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" s="6"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>0.91329000000000005</v>
@@ -1090,12 +1103,12 @@
         <v>0.94700410000000002</v>
       </c>
       <c r="E19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>26</v>
       </c>
       <c r="B20" s="7">
         <v>0.91571999999999998</v>
@@ -1107,9 +1120,9 @@
         <v>0.94724229999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>0.91281000000000001</v>
@@ -1119,6 +1132,23 @@
       </c>
       <c r="D21">
         <v>0.94708349999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="1" customFormat="1">
+      <c r="A23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.92666999999999999</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.91173470000000001</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1132,7 +1162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -1148,102 +1178,102 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:1" s="8" customFormat="1">
       <c r="A8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1254,7 +1284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A53"/>
   <sheetViews>
@@ -1269,267 +1299,267 @@
   <sheetData>
     <row r="1" spans="1:1" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update study9 and study10.R to impute variable
</commit_message>
<xml_diff>
--- a/kaggleCompetition/指标.xlsx
+++ b/kaggleCompetition/指标.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="20415" windowHeight="7770"/>
@@ -367,7 +367,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00000_ "/>
   </numFmts>
@@ -507,7 +507,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -581,7 +581,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -616,7 +615,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -792,12 +790,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1151,6 +1149,9 @@
         <v>104</v>
       </c>
     </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F9:F14"/>
@@ -1162,7 +1163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -1284,7 +1285,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:A53"/>
   <sheetViews>

</xml_diff>